<commit_message>
fixed template,  remove version
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/TeploSilaWeb/TeplosilaWeb/Content/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6EDBE64F-2CC8-4EF0-9CCF-1B5E5FF6BF81}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,79 +575,79 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,12 +1015,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1038,16 +1038,16 @@
       <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1062,21 +1062,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1091,21 +1091,21 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1120,21 +1120,21 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1149,12 +1149,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1176,19 +1176,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1203,21 +1203,21 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="7"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="29"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="2"/>
@@ -1234,17 +1234,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="29"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="19"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
@@ -1261,17 +1261,17 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="29"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
       <c r="J11" s="19"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2"/>
@@ -1288,17 +1288,17 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="29"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
       <c r="J12" s="19"/>
       <c r="K12" s="18" t="s">
         <v>43</v>
@@ -1317,21 +1317,21 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="40" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="40" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="42"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="28"/>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1346,26 +1346,26 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="4" t="s">
         <v>43</v>
       </c>
@@ -1383,24 +1383,24 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="4" t="s">
         <v>43</v>
       </c>
@@ -1418,26 +1418,26 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="4" t="s">
         <v>43</v>
       </c>
@@ -1455,24 +1455,24 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="4" t="s">
         <v>43</v>
       </c>
@@ -1490,20 +1490,20 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="4"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1519,20 +1519,20 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
       <c r="K19" s="4"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1548,13 +1548,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1575,21 +1575,21 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="28" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="33"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1604,21 +1604,21 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="28" t="s">
+      <c r="B22" s="25"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="33"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="35"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1633,13 +1633,13 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1660,19 +1660,19 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -1687,19 +1687,19 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1811,13 +1811,13 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -1838,33 +1838,33 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26" t="s">
+      <c r="D30" s="40"/>
+      <c r="E30" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G30" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26" t="s">
+      <c r="H30" s="40"/>
+      <c r="I30" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="26" t="s">
+      <c r="J30" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="K30" s="26" t="s">
+      <c r="K30" s="40" t="s">
         <v>61</v>
       </c>
       <c r="L30" s="2"/>
@@ -1880,26 +1880,26 @@
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
     </row>
-    <row r="31" spans="1:23" s="1" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
+    <row r="31" spans="1:23" s="1" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="11" t="s">
         <v>60</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
       <c r="G31" s="11" t="s">
         <v>59</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1939,19 +1939,19 @@
       <c r="W32" s="2"/>
     </row>
     <row r="33" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -1966,19 +1966,19 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -1993,19 +1993,19 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2047,11 +2047,11 @@
     <row r="37" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="17"/>
       <c r="H37" s="16" t="s">
         <v>44</v>
@@ -2075,11 +2075,11 @@
     <row r="38" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="17"/>
       <c r="H38" s="16" t="s">
         <v>44</v>
@@ -2103,11 +2103,11 @@
     <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
       <c r="G39" s="17"/>
       <c r="H39" s="16" t="s">
         <v>44</v>
@@ -2131,11 +2131,11 @@
     <row r="40" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
       <c r="G40" s="17"/>
       <c r="H40" s="16" t="s">
         <v>66</v>
@@ -3013,30 +3013,44 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E25:K25"/>
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:B8"/>
@@ -3053,44 +3067,30 @@
     <mergeCell ref="K30:K31"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed image in excel and fixed css
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/TeploSilaWeb/TeplosilaWeb/Content/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8549556-4451-4714-9B2B-8406D7EA2C2D}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{603B318F-C2B8-4128-A29D-8540DDA239B6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,80 +575,80 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30:J31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,12 +1015,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1038,16 +1038,16 @@
       <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1062,21 +1062,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1091,21 +1091,21 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1120,21 +1120,21 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1149,12 +1149,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1176,19 +1176,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1203,21 +1203,21 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="7"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="29"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="2"/>
@@ -1234,17 +1234,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="29"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="19"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
@@ -1261,17 +1261,17 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="29"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
       <c r="J11" s="19"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2"/>
@@ -1288,17 +1288,17 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="29"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
       <c r="J12" s="19"/>
       <c r="K12" s="18" t="s">
         <v>43</v>
@@ -1317,21 +1317,21 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="41" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="41" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="43"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="28"/>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1346,26 +1346,26 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="4" t="s">
         <v>43</v>
       </c>
@@ -1383,24 +1383,24 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="4" t="s">
         <v>43</v>
       </c>
@@ -1418,26 +1418,26 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="4" t="s">
         <v>43</v>
       </c>
@@ -1455,24 +1455,24 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="4" t="s">
         <v>43</v>
       </c>
@@ -1490,20 +1490,20 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="4"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1519,20 +1519,20 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
       <c r="K19" s="4"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1548,13 +1548,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1575,21 +1575,21 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="28" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="33"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1604,21 +1604,21 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="28" t="s">
+      <c r="B22" s="25"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="33"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="35"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1633,13 +1633,13 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1660,19 +1660,19 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -1687,19 +1687,19 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1785,7 +1785,7 @@
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
     </row>
-    <row r="28" spans="1:23" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1811,13 +1811,13 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -1838,33 +1838,33 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26" t="s">
+      <c r="D30" s="40"/>
+      <c r="E30" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G30" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26" t="s">
+      <c r="H30" s="40"/>
+      <c r="I30" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="26" t="s">
+      <c r="J30" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="K30" s="26" t="s">
+      <c r="K30" s="40" t="s">
         <v>61</v>
       </c>
       <c r="L30" s="2"/>
@@ -1881,25 +1881,25 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="11" t="s">
         <v>60</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
       <c r="G31" s="11" t="s">
         <v>59</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1939,19 +1939,19 @@
       <c r="W32" s="2"/>
     </row>
     <row r="33" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -1966,19 +1966,19 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -1993,19 +1993,19 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2047,11 +2047,11 @@
     <row r="37" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="17"/>
       <c r="H37" s="16" t="s">
         <v>44</v>
@@ -2075,11 +2075,11 @@
     <row r="38" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="17"/>
       <c r="H38" s="16" t="s">
         <v>44</v>
@@ -2103,11 +2103,11 @@
     <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
       <c r="G39" s="17"/>
       <c r="H39" s="16" t="s">
         <v>44</v>
@@ -2131,11 +2131,11 @@
     <row r="40" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
       <c r="G40" s="17"/>
       <c r="H40" s="16" t="s">
         <v>65</v>
@@ -3013,30 +3013,44 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E25:K25"/>
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:B8"/>
@@ -3053,44 +3067,30 @@
     <mergeCell ref="K30:K31"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added steam in TRV
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/TeploSilaWeb/TeplosilaWeb/Content/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81F01F72-0533-43DE-B28B-2E3F2C35DA48}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D188564A-C31E-4C5F-9533-A497EDE38EBC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Марка регулирующего клапана</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>Пропускная способность Kvs, м³/ч</t>
+  </si>
+  <si>
+    <t>Датчики температуры поставляются отдельно.</t>
   </si>
 </sst>
 </file>
@@ -539,9 +542,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -551,9 +551,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -575,80 +572,86 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,12 +1018,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1035,7 +1038,7 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="31"/>
@@ -1062,21 +1065,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1091,21 +1094,21 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1120,21 +1123,21 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1149,12 +1152,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1176,19 +1179,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1203,21 +1206,21 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="7"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="29"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="2"/>
@@ -1234,18 +1237,18 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="19"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1261,18 +1264,18 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="19"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="17"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1288,19 +1291,19 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="18" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="16" t="s">
         <v>42</v>
       </c>
       <c r="L12" s="2"/>
@@ -1317,21 +1320,21 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="41" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="41" t="s">
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="43"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1346,26 +1349,26 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
       <c r="K14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1383,24 +1386,24 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="15" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
       <c r="K15" s="4" t="s">
         <v>42</v>
       </c>
@@ -1418,26 +1421,26 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
       <c r="K16" s="4" t="s">
         <v>42</v>
       </c>
@@ -1455,24 +1458,24 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="15" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="25"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
       <c r="K17" s="4" t="s">
         <v>42</v>
       </c>
@@ -1490,20 +1493,20 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
       <c r="K18" s="4"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1519,20 +1522,20 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
       <c r="K19" s="4"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1548,13 +1551,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1575,19 +1578,19 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="31"/>
       <c r="D21" s="32"/>
       <c r="E21" s="33"/>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="29"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
       <c r="J21" s="31"/>
       <c r="K21" s="33"/>
       <c r="L21" s="2"/>
@@ -1604,19 +1607,19 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="29"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
       <c r="E22" s="33"/>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="29"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
       <c r="J22" s="31"/>
       <c r="K22" s="33"/>
       <c r="L22" s="2"/>
@@ -1633,13 +1636,13 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1660,19 +1663,19 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -1687,19 +1690,19 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1739,37 +1742,37 @@
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="1:23" s="1" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="10" t="s">
         <v>76</v>
       </c>
       <c r="L27" s="2"/>
@@ -1786,17 +1789,17 @@
       <c r="W27" s="2"/>
     </row>
     <row r="28" spans="1:23" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -1811,19 +1814,19 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1838,33 +1841,33 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26" t="s">
+      <c r="D30" s="38"/>
+      <c r="E30" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G30" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26" t="s">
+      <c r="H30" s="38"/>
+      <c r="I30" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="26" t="s">
+      <c r="J30" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="K30" s="26" t="s">
+      <c r="K30" s="38" t="s">
         <v>60</v>
       </c>
       <c r="L30" s="2"/>
@@ -1881,25 +1884,25 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="11" t="s">
+      <c r="A31" s="38"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="11" t="s">
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1914,17 +1917,17 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" spans="1:23" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -1939,19 +1942,19 @@
       <c r="W32" s="2"/>
     </row>
     <row r="33" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="41"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -1966,19 +1969,19 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -1993,19 +1996,19 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2019,18 +2022,20 @@
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
     </row>
-    <row r="36" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
+    <row r="36" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2047,15 +2052,6 @@
     <row r="37" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="D37" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="16" t="s">
-        <v>43</v>
-      </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2075,13 +2071,13 @@
     <row r="38" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-      <c r="D38" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="16" t="s">
+      <c r="D38" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="14" t="s">
         <v>43</v>
       </c>
       <c r="I38" s="3"/>
@@ -2103,13 +2099,13 @@
     <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="D39" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="16" t="s">
+      <c r="D39" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="14" t="s">
         <v>43</v>
       </c>
       <c r="I39" s="3"/>
@@ -2131,14 +2127,14 @@
     <row r="40" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="D40" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="16" t="s">
-        <v>64</v>
+      <c r="D40" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
@@ -2159,12 +2155,16 @@
     <row r="41" spans="1:23" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="14" t="s">
+        <v>64</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2262,10 +2262,6 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
@@ -2282,10 +2278,6 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
@@ -2302,10 +2294,6 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
@@ -2322,11 +2310,6 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
@@ -3012,62 +2995,17 @@
       <c r="W75" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="78">
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:K24"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="K30:K31"/>
+  <mergeCells count="79">
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="D37:F37"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="I16:J16"/>
@@ -3083,14 +3021,60 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:K24"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed image and css and radiobutton
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/TeploSilaWeb/TeplosilaWeb/Content/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8584385C-E5B1-4613-84A3-73C8C4C9A50B}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A594953C-B61D-46BD-BC36-616753D767FB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Марка регулирующего клапана</t>
   </si>
@@ -74,21 +74,6 @@
     <t>Внешний авторитет клапана</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Предельно допустимый перепад давлений на клапане </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>ΔPпред, бар</t>
-    </r>
-  </si>
-  <si>
     <t>Дата расчета:</t>
   </si>
   <si>
@@ -120,9 +105,6 @@
   </si>
   <si>
     <t>Управление:</t>
-  </si>
-  <si>
-    <t>Наличие датчика положения 4-20 mA:</t>
   </si>
   <si>
     <t>Наличие возвратного механизма:</t>
@@ -267,10 +249,6 @@
     <t>Потребл. мощность, W</t>
   </si>
   <si>
-    <t>Наличие датчика положения
-4-20 mA</t>
-  </si>
-  <si>
     <t>Область применения:</t>
   </si>
   <si>
@@ -306,10 +284,6 @@
 не более</t>
   </si>
   <si>
-    <t>4-20 mA
-(2-10 V)</t>
-  </si>
-  <si>
     <t>Оптимальная скорость в выходном сечении клапана: 2-3 м/с для ИТП; 2-5 м/с для ЦТП.</t>
   </si>
   <si>
@@ -321,9 +295,6 @@
     <t>Максимальная температура среды через клапан Т1=</t>
   </si>
   <si>
-    <t>Обозначение электро- привода</t>
-  </si>
-  <si>
     <t>Наличие возврат- ного меха- низма</t>
   </si>
   <si>
@@ -334,6 +305,21 @@
   </si>
   <si>
     <t>Наличие функции регулирования температуры (датчик температуры подключается к электроприводу):</t>
+  </si>
+  <si>
+    <t>Предельно допустимый перепад давлений на клапане ΔPпред, бар</t>
+  </si>
+  <si>
+    <t>Наличие датчика положения 0(4)-20 mA:</t>
+  </si>
+  <si>
+    <t>0(4)-20 mA,
+0(2)-10 V</t>
+  </si>
+  <si>
+    <t>Наличие датчика положения
+0(4)-20 mA,
+0(2)-10 V</t>
   </si>
 </sst>
 </file>
@@ -613,23 +599,92 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -641,75 +696,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -740,9 +726,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>493712</xdr:colOff>
+      <xdr:colOff>422275</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>20360</xdr:rowOff>
+      <xdr:rowOff>16550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1049,18 +1035,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:I21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="7.109375" style="3" customWidth="1"/>
     <col min="8" max="9" width="9.88671875" style="3" customWidth="1"/>
     <col min="10" max="10" width="7.5546875" style="3" customWidth="1"/>
@@ -1077,12 +1063,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="H2" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1096,20 +1082,20 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+        <v>9</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1124,21 +1110,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
+      <c r="A4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1153,21 +1139,21 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="A5" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1182,21 +1168,21 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
+      <c r="A6" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1211,12 +1197,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
+      <c r="A7" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1238,19 +1224,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
+      <c r="A8" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1265,21 +1251,21 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="21"/>
+      <c r="A9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="27"/>
       <c r="E9" s="7"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="24"/>
+      <c r="G9" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="29"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="2"/>
@@ -1296,17 +1282,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
+      <c r="A10" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="29"/>
       <c r="J10" s="14"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
@@ -1323,17 +1309,17 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
+      <c r="A11" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="29"/>
       <c r="J11" s="14"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2"/>
@@ -1350,20 +1336,20 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
+      <c r="A12" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="29"/>
       <c r="J12" s="14"/>
       <c r="K12" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1379,21 +1365,21 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1408,28 +1394,28 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
       <c r="K14" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="5"/>
@@ -1445,26 +1431,26 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="21"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="27"/>
       <c r="D15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="32"/>
       <c r="K15" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="5"/>
@@ -1480,28 +1466,28 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="21"/>
+      <c r="A16" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="27"/>
       <c r="D16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="31"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="5"/>
@@ -1517,26 +1503,26 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="21"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="27"/>
       <c r="D17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="32"/>
       <c r="K17" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="5"/>
@@ -1552,20 +1538,20 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
+      <c r="A18" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="29"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="32"/>
       <c r="K18" s="4"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1581,20 +1567,20 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="A19" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
       <c r="K19" s="4"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1610,13 +1596,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="A20" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1637,19 +1623,19 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="20"/>
+      <c r="A21" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="32"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1664,21 +1650,21 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="34"/>
+      <c r="A22" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="37"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1693,21 +1679,21 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="34"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="37"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1722,13 +1708,13 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
+      <c r="A24" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -1749,19 +1735,19 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="34"/>
+      <c r="A25" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="37"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1776,19 +1762,19 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="34"/>
+      <c r="A26" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="37"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1802,7 +1788,7 @@
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
     </row>
-    <row r="27" spans="1:23" s="1" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1827,7 +1813,7 @@
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
     </row>
-    <row r="28" spans="1:23" s="1" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" s="1" customFormat="1" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>0</v>
       </c>
@@ -1835,31 +1821,29 @@
         <v>1</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="26"/>
+      <c r="F28" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="G28" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="H28" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="I28" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="17" t="s">
-        <v>8</v>
-      </c>
       <c r="J28" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K28" s="17" t="s">
         <v>5</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>76</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -1874,12 +1858,12 @@
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
     </row>
-    <row r="29" spans="1:23" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" s="1" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -1900,13 +1884,13 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
+      <c r="A30" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -1927,34 +1911,34 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="50" t="s">
+      <c r="A31" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="26"/>
+      <c r="E31" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="51"/>
-      <c r="E31" s="41" t="s">
+      <c r="G31" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="H31" s="51"/>
-      <c r="I31" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="K31" s="41" t="s">
-        <v>60</v>
+      <c r="H31" s="26"/>
+      <c r="I31" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -1970,25 +1954,25 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" spans="1:23" s="1" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
+        <v>64</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
       <c r="G32" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
+        <v>78</v>
+      </c>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2027,20 +2011,20 @@
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
     </row>
-    <row r="34" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
+    <row r="34" spans="1:23" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2055,19 +2039,19 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
+      <c r="A35" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2081,20 +2065,20 @@
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
     </row>
-    <row r="36" spans="1:23" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
+    <row r="36" spans="1:23" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2108,20 +2092,20 @@
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
     </row>
-    <row r="37" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
+    <row r="37" spans="1:23" s="1" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2135,7 +2119,7 @@
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
     </row>
-    <row r="38" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="I38" s="15"/>
@@ -2157,14 +2141,14 @@
     <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
-      <c r="D39" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="23"/>
-      <c r="F39" s="24"/>
+      <c r="D39" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="30"/>
+      <c r="F39" s="29"/>
       <c r="G39" s="18"/>
       <c r="H39" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -2185,14 +2169,14 @@
     <row r="40" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
-      <c r="D40" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="24"/>
+      <c r="D40" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="30"/>
+      <c r="F40" s="29"/>
       <c r="G40" s="18"/>
       <c r="H40" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
@@ -2213,14 +2197,14 @@
     <row r="41" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
-      <c r="D41" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="24"/>
+      <c r="D41" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="30"/>
+      <c r="F41" s="29"/>
       <c r="G41" s="18"/>
       <c r="H41" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
@@ -2242,14 +2226,14 @@
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
+      <c r="D42" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" s="41"/>
+      <c r="F42" s="42"/>
       <c r="G42" s="18"/>
       <c r="H42" s="16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -3081,7 +3065,74 @@
       <c r="W76" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="81">
+  <mergeCells count="83">
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A37:K37"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="F5:I5"/>
@@ -3098,71 +3149,6 @@
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="F22:I22"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed file, validators and table
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/TeploSilaWeb/TeplosilaWeb/Content/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A594953C-B61D-46BD-BC36-616753D767FB}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{9ED26EFC-5770-46C3-B258-2113F5CC8C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC90DEE6-ECDD-43DF-A6F0-5E75E10911DA}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,7 +728,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>422275</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>16550</xdr:rowOff>
+      <xdr:rowOff>20360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:D31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1986,7 +1986,7 @@
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
     </row>
-    <row r="33" spans="1:23" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>

</xml_diff>

<commit_message>
fix 17.10.2023 cost 0.5 h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/TeploSilaWeb/TeplosilaWeb/Content/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\ТЗ программа подбора TRV, RDT\ТЗ клапаны TRV\Бланки расчетных листов\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_1DE73C2019F529DF09AFA0E86561F075689B104F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{755F5FD4-1992-4FAF-BFB8-A3D4AA9FA061}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="11715"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -116,9 +115,6 @@
     <t>Максимальное рабочее давление:</t>
   </si>
   <si>
-    <t>Рекомендуемая скорость управления для электроприводов TW500, TW1001, TW3000 - 2 сек/мм (30 мм/мин).</t>
-  </si>
-  <si>
     <t>Тепловая мощность:</t>
   </si>
   <si>
@@ -275,11 +271,6 @@
     <t>Оптимальная скорость в выходном сечении клапана: 2-3 м/с для ИТП; 2-5 м/с для ЦТП.</t>
   </si>
   <si>
-    <t>Рекомендуемая скорость управления для электроприводов TSL-1600, TSL-2200, TSL-3000:
-- системы отопления и вентиляции: для Ду15-50 мм - 8 сек/мм (7,5 мм/мин); для Ду65-100 - 6 сек/мм (10 мм/мин);
-- система горячего водоснабжения: для Ду15-50 мм - 4 сек/мм (15 мм/мин); для Ду65-100 - 2,4 сек/мм (25 мм/мин).</t>
-  </si>
-  <si>
     <t>Максимальная температура среды через клапан Т1=</t>
   </si>
   <si>
@@ -311,12 +302,20 @@
   </si>
   <si>
     <t>Потери давления на регулируемом участке (без учета регулирующего клапана) ΔPру'=</t>
+  </si>
+  <si>
+    <t>Рекомендуемая скорость управления для электропривода TW5000 - 2 сек/мм (30 мм/мин).</t>
+  </si>
+  <si>
+    <t>Рекомендуемая скорость управления для электроприводов TSL:
+- системы отопления и вентиляции: для Ду15-50 мм - 8 сек/мм (7,5 мм/мин); для Ду65-200 - 6 сек/мм (10 мм/мин);
+- система горячего водоснабжения: для Ду15-50 мм - 4 сек/мм (15 мм/мин); для Ду65-200 - 2,4 сек/мм (25 мм/мин).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -581,17 +580,92 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -602,83 +676,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,11 +1013,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:E23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,17 +1036,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1057,12 +1056,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1080,16 +1079,16 @@
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1104,21 +1103,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1133,21 +1132,21 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36" t="s">
+      <c r="A5" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1162,19 +1161,19 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
+      <c r="A6" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1189,12 +1188,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1216,19 +1215,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1243,17 +1242,17 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
+      <c r="A9" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="2"/>
@@ -1270,17 +1269,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
+      <c r="A10" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="14"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
@@ -1297,17 +1296,17 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21"/>
+      <c r="A11" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="14"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2"/>
@@ -1324,20 +1323,20 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="A12" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="14"/>
       <c r="K12" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1353,21 +1352,21 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="23" t="s">
+      <c r="A13" s="33"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1382,28 +1381,28 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="22"/>
+      <c r="A14" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="30"/>
       <c r="D14" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="34"/>
       <c r="G14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="28"/>
+        <v>33</v>
+      </c>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
       <c r="K14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="5"/>
@@ -1419,26 +1418,26 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="22"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="30"/>
       <c r="D15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="28"/>
+        <v>30</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
       <c r="G15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="26"/>
-      <c r="J15" s="28"/>
+        <v>32</v>
+      </c>
+      <c r="I15" s="33"/>
+      <c r="J15" s="34"/>
       <c r="K15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="5"/>
@@ -1454,28 +1453,28 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="22"/>
+      <c r="A16" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="30"/>
       <c r="D16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="28"/>
+        <v>34</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="34"/>
       <c r="G16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="28"/>
+        <v>36</v>
+      </c>
+      <c r="I16" s="33"/>
+      <c r="J16" s="34"/>
       <c r="K16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="5"/>
@@ -1491,26 +1490,26 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="22"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="30"/>
       <c r="D17" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="28"/>
+        <v>35</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
       <c r="G17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="5"/>
@@ -1526,20 +1525,20 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="28"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="34"/>
       <c r="K18" s="4"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1555,20 +1554,20 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22" t="s">
+      <c r="A19" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
       <c r="K19" s="4"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1584,13 +1583,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
+      <c r="A20" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1611,19 +1610,19 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="28"/>
+      <c r="A21" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="34"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1638,21 +1637,21 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="28"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="34"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1667,21 +1666,21 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="19" t="s">
+      <c r="B23" s="32"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="28"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="34"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1696,13 +1695,13 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -1723,19 +1722,19 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="34"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1750,19 +1749,19 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="34"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1809,12 +1808,12 @@
         <v>1</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="49"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="17" t="s">
         <v>7</v>
       </c>
@@ -1828,7 +1827,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>5</v>
@@ -1850,8 +1849,8 @@
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="49"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -1872,13 +1871,13 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
+      <c r="A30" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -1899,34 +1898,34 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="48" t="s">
+      <c r="A31" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="41" t="s">
+      <c r="F31" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="41" t="s">
+      <c r="G31" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" s="49"/>
-      <c r="I31" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="J31" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="K31" s="41" t="s">
-        <v>54</v>
+      <c r="H31" s="29"/>
+      <c r="I31" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="J31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -1942,25 +1941,25 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" spans="1:23" s="1" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
+        <v>59</v>
+      </c>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
+        <v>72</v>
+      </c>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2000,19 +1999,19 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
+      <c r="A34" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2027,19 +2026,19 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="45"/>
+      <c r="A35" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2054,19 +2053,19 @@
       <c r="W35" s="2"/>
     </row>
     <row r="36" spans="1:23" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
+      <c r="A36" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2081,19 +2080,19 @@
       <c r="W36" s="2"/>
     </row>
     <row r="37" spans="1:23" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="51"/>
+      <c r="A37" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2129,14 +2128,14 @@
     <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
-      <c r="D39" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="21"/>
+      <c r="D39" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="36"/>
+      <c r="F39" s="32"/>
       <c r="G39" s="18"/>
       <c r="H39" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -2157,14 +2156,14 @@
     <row r="40" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
-      <c r="D40" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
+      <c r="D40" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="36"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="18"/>
       <c r="H40" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
@@ -2185,14 +2184,14 @@
     <row r="41" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
-      <c r="D41" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
+      <c r="D41" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="36"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="18"/>
       <c r="H41" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
@@ -2214,14 +2213,14 @@
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
+      <c r="D42" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="41"/>
+      <c r="F42" s="42"/>
       <c r="G42" s="18"/>
       <c r="H42" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -3054,6 +3053,70 @@
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:F18"/>
     <mergeCell ref="C6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A37:K37"/>
@@ -3070,70 +3133,6 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix 16.04.2024 price 9 h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\ТЗ программа подбора TRV, RDT\ТЗ клапаны TRV\Бланки расчетных листов\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A90D8F0-59F5-4BDF-B585-C27B0E2B9B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="11715"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -103,9 +104,6 @@
     <t>Управление:</t>
   </si>
   <si>
-    <t>Наличие возвратного механизма:</t>
-  </si>
-  <si>
     <t>Результат расчета регулирующего клапана</t>
   </si>
   <si>
@@ -274,9 +272,6 @@
     <t>Максимальная температура среды через клапан Т1=</t>
   </si>
   <si>
-    <t>Наличие возврат- ного меха- низма</t>
-  </si>
-  <si>
     <t>Пропускная способность Kvs, м³/ч</t>
   </si>
   <si>
@@ -310,12 +305,18 @@
     <t>Рекомендуемая скорость управления для электроприводов TSL:
 - системы отопления и вентиляции: для Ду15-50 мм - 8 сек/мм (7,5 мм/мин); для Ду65-200 - 6 сек/мм (10 мм/мин);
 - система горячего водоснабжения: для Ду15-50 мм - 4 сек/мм (15 мм/мин); для Ду65-200 - 2,4 сек/мм (25 мм/мин).</t>
+  </si>
+  <si>
+    <t>Наличие функции безопасности:</t>
+  </si>
+  <si>
+    <t>Наличие функции безопас-ности</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,6 +581,45 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -589,95 +629,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1013,40 +1014,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="3" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="3" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="3" customWidth="1"/>
     <col min="12" max="23" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1056,12 +1057,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="47"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1079,16 +1080,16 @@
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="34"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1103,21 +1104,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1132,21 +1133,21 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25" t="s">
+      <c r="A5" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1161,19 +1162,19 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
+      <c r="A6" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1188,12 +1189,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1215,19 +1216,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1242,17 +1243,17 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="32"/>
+      <c r="A9" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="2"/>
@@ -1269,17 +1270,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="32"/>
+      <c r="A10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="14"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
@@ -1296,17 +1297,17 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="32"/>
+      <c r="A11" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="14"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2"/>
@@ -1323,20 +1324,20 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="32"/>
+      <c r="A12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="14"/>
       <c r="K12" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1352,21 +1353,21 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="48" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="50"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1381,28 +1382,28 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="30"/>
+      <c r="A14" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="22"/>
       <c r="D14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
+        <v>30</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="28"/>
       <c r="G14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
+        <v>32</v>
+      </c>
+      <c r="I14" s="26"/>
+      <c r="J14" s="28"/>
       <c r="K14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="5"/>
@@ -1418,26 +1419,26 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="30"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="22"/>
       <c r="D15" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
+        <v>29</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
+        <v>31</v>
+      </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="28"/>
       <c r="K15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="5"/>
@@ -1453,28 +1454,28 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="30"/>
+      <c r="A16" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="22"/>
       <c r="D16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
+        <v>33</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34"/>
+        <v>35</v>
+      </c>
+      <c r="I16" s="26"/>
+      <c r="J16" s="28"/>
       <c r="K16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="5"/>
@@ -1490,26 +1491,26 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="30"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="22"/>
       <c r="D17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34"/>
+        <v>34</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="26"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="5"/>
@@ -1525,20 +1526,20 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="28"/>
       <c r="K18" s="4"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1554,20 +1555,20 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30" t="s">
+      <c r="A19" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
       <c r="K19" s="4"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1583,13 +1584,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
+      <c r="A20" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1610,19 +1611,19 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="34"/>
+      <c r="A21" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="28"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1637,21 +1638,21 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="34"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="28"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1666,21 +1667,21 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="34"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="28"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1695,13 +1696,13 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
+      <c r="A24" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -1722,19 +1723,19 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
+      <c r="A25" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="34"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1749,19 +1750,19 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="A26" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="34"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1808,12 +1809,12 @@
         <v>1</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="17" t="s">
         <v>7</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>5</v>
@@ -1849,8 +1850,8 @@
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="49"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -1871,13 +1872,13 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
+      <c r="A30" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -1898,34 +1899,34 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="28" t="s">
+      <c r="A31" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="49"/>
+      <c r="E31" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="26" t="s">
+      <c r="F31" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="G31" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="H31" s="29"/>
-      <c r="I31" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="J31" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="K31" s="26" t="s">
-        <v>53</v>
+      <c r="H31" s="49"/>
+      <c r="I31" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="J31" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="K31" s="41" t="s">
+        <v>52</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -1941,25 +1942,25 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" spans="1:23" s="1" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
+        <v>58</v>
+      </c>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
+        <v>70</v>
+      </c>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -1999,19 +2000,19 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
+      <c r="A34" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2026,19 +2027,19 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
+      <c r="A35" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2053,19 +2054,19 @@
       <c r="W35" s="2"/>
     </row>
     <row r="36" spans="1:23" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
+      <c r="A36" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2080,19 +2081,19 @@
       <c r="W36" s="2"/>
     </row>
     <row r="37" spans="1:23" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
+      <c r="A37" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2128,14 +2129,14 @@
     <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
-      <c r="D39" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="32"/>
+      <c r="D39" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="18"/>
       <c r="H39" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -2156,14 +2157,14 @@
     <row r="40" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
-      <c r="D40" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="36"/>
-      <c r="F40" s="32"/>
+      <c r="D40" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
       <c r="G40" s="18"/>
       <c r="H40" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
@@ -2184,14 +2185,14 @@
     <row r="41" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
-      <c r="D41" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="32"/>
+      <c r="D41" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
       <c r="G41" s="18"/>
       <c r="H41" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
@@ -2213,14 +2214,14 @@
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="E42" s="41"/>
-      <c r="F42" s="42"/>
+      <c r="D42" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="38"/>
+      <c r="F42" s="39"/>
       <c r="G42" s="18"/>
       <c r="H42" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -3053,27 +3054,49 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A26:D26"/>
     <mergeCell ref="D42:F42"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:B8"/>
@@ -3090,49 +3113,27 @@
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix 18.04.2024 price 10h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A90D8F0-59F5-4BDF-B585-C27B0E2B9B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C568183-367F-4B39-9F2D-4388C854659C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,13 +33,7 @@
     <t>Номинальный диаметр DN, мм</t>
   </si>
   <si>
-    <t>Качество регулирования</t>
-  </si>
-  <si>
     <t>Скорость в выходном сечении клапана V, м/с</t>
-  </si>
-  <si>
-    <t>Шум, некачественное регулирование</t>
   </si>
   <si>
     <t>Кавитация</t>
@@ -311,6 +305,12 @@
   </si>
   <si>
     <t>Наличие функции безопас-ности</t>
+  </si>
+  <si>
+    <t>Шум, колебатель-ный режим</t>
+  </si>
+  <si>
+    <t>Качество регули-рования</t>
   </si>
 </sst>
 </file>
@@ -581,17 +581,92 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -602,83 +677,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31:K32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,17 +1037,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1057,12 +1057,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="H2" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1078,18 +1078,18 @@
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+        <v>7</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1104,21 +1104,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
+      <c r="A4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1133,21 +1133,21 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="A5" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1162,19 +1162,19 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
+      <c r="A6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1189,12 +1189,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
+      <c r="A7" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1216,19 +1216,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
+      <c r="A8" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1243,17 +1243,17 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
+      <c r="A9" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="2"/>
@@ -1270,17 +1270,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
+      <c r="A10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="14"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
@@ -1297,17 +1297,17 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21"/>
+      <c r="A11" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="14"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2"/>
@@ -1324,20 +1324,20 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="A12" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="14"/>
       <c r="K12" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1353,21 +1353,21 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1382,28 +1382,28 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="28"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
       <c r="K14" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="5"/>
@@ -1419,26 +1419,26 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="22"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="30"/>
       <c r="D15" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="26"/>
-      <c r="J15" s="28"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="34"/>
       <c r="K15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="5"/>
@@ -1454,28 +1454,28 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="22"/>
+      <c r="A16" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="30"/>
       <c r="D16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="33"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="5"/>
@@ -1491,26 +1491,26 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="22"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="30"/>
       <c r="D17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="28"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
       <c r="K17" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="5"/>
@@ -1526,20 +1526,20 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="28"/>
+      <c r="A18" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="34"/>
       <c r="K18" s="4"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1555,20 +1555,20 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="A19" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
       <c r="K19" s="4"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1584,13 +1584,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
+      <c r="A20" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1611,19 +1611,19 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="28"/>
+      <c r="A21" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="34"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1638,21 +1638,21 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="28"/>
+      <c r="A22" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="34"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1667,21 +1667,21 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="28"/>
+      <c r="A23" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="34"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1696,13 +1696,13 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
+      <c r="A24" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -1723,19 +1723,19 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="34"/>
+      <c r="A25" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1750,19 +1750,19 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="34"/>
+      <c r="A26" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1809,29 +1809,29 @@
         <v>1</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="49"/>
+        <v>63</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="29"/>
       <c r="F28" s="17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G28" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="I28" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="17" t="s">
         <v>3</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>5</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -1850,8 +1850,8 @@
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="49"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -1872,13 +1872,13 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
+      <c r="A30" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -1899,34 +1899,34 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="48" t="s">
+      <c r="A31" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="41" t="s">
+      <c r="G31" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="G31" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="H31" s="49"/>
-      <c r="I31" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="J31" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="K31" s="41" t="s">
-        <v>52</v>
+      <c r="H31" s="29"/>
+      <c r="I31" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="J31" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="K31" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -1942,25 +1942,25 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" spans="1:23" s="1" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
+        <v>56</v>
+      </c>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
+        <v>68</v>
+      </c>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2000,19 +2000,19 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
+      <c r="A34" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2027,19 +2027,19 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="45"/>
+      <c r="A35" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2054,19 +2054,19 @@
       <c r="W35" s="2"/>
     </row>
     <row r="36" spans="1:23" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
+      <c r="A36" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2081,19 +2081,19 @@
       <c r="W36" s="2"/>
     </row>
     <row r="37" spans="1:23" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="51"/>
+      <c r="A37" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2129,14 +2129,14 @@
     <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
-      <c r="D39" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="21"/>
+      <c r="D39" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="36"/>
+      <c r="F39" s="32"/>
       <c r="G39" s="18"/>
       <c r="H39" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
@@ -2157,14 +2157,14 @@
     <row r="40" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
-      <c r="D40" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
+      <c r="D40" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="36"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="18"/>
       <c r="H40" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
@@ -2185,14 +2185,14 @@
     <row r="41" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
-      <c r="D41" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
+      <c r="D41" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" s="36"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="18"/>
       <c r="H41" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
@@ -2214,14 +2214,14 @@
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="39"/>
+      <c r="D42" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="41"/>
+      <c r="F42" s="42"/>
       <c r="G42" s="18"/>
       <c r="H42" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -3054,6 +3054,70 @@
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:F18"/>
     <mergeCell ref="C6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A37:K37"/>
@@ -3070,70 +3134,6 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix2 18.04.2024 price 10h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRV.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C568183-367F-4B39-9F2D-4388C854659C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C152528-0328-4486-9421-2CD3A7AA86AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,10 +307,10 @@
     <t>Наличие функции безопас-ности</t>
   </si>
   <si>
-    <t>Шум, колебатель-ный режим</t>
-  </si>
-  <si>
     <t>Качество регули-рования</t>
+  </si>
+  <si>
+    <t>Шум, колебательный режим</t>
   </si>
 </sst>
 </file>
@@ -581,6 +581,45 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -590,95 +629,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:W76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,17 +1037,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1057,12 +1057,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="47"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1080,16 +1080,16 @@
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="34"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1104,21 +1104,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1133,21 +1133,21 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1162,19 +1162,19 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1189,12 +1189,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1216,19 +1216,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1243,17 +1243,17 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="32"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="2"/>
@@ -1270,17 +1270,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="32"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="14"/>
       <c r="K10" s="6"/>
       <c r="L10" s="2"/>
@@ -1297,17 +1297,17 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="32"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="14"/>
       <c r="K11" s="6"/>
       <c r="L11" s="2"/>
@@ -1324,17 +1324,17 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="32"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="14"/>
       <c r="K12" s="13" t="s">
         <v>35</v>
@@ -1353,21 +1353,21 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="48" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="48" t="s">
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="50"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1382,26 +1382,26 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="28"/>
       <c r="G14" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="28"/>
       <c r="K14" s="4" t="s">
         <v>35</v>
       </c>
@@ -1419,24 +1419,24 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="28"/>
       <c r="K15" s="4" t="s">
         <v>35</v>
       </c>
@@ -1454,26 +1454,26 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="30"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="28"/>
       <c r="K16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1491,24 +1491,24 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="4" t="s">
         <v>35</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="28"/>
       <c r="K17" s="4" t="s">
         <v>35</v>
       </c>
@@ -1526,20 +1526,20 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="31" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="28"/>
       <c r="K18" s="4"/>
       <c r="L18" s="2"/>
       <c r="M18" s="5"/>
@@ -1555,20 +1555,20 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
       <c r="K19" s="4"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1584,13 +1584,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1611,19 +1611,19 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="34"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="28"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1638,21 +1638,21 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="31" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="34"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="28"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1667,21 +1667,21 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="31" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="34"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="28"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1696,13 +1696,13 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -1723,19 +1723,19 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="34"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1750,19 +1750,19 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="34"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1811,21 +1811,21 @@
       <c r="C28" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="17" t="s">
         <v>5</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H28" s="17" t="s">
         <v>2</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J28" s="17" t="s">
         <v>66</v>
@@ -1850,8 +1850,8 @@
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="49"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -1872,13 +1872,13 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -1899,33 +1899,33 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="26" t="s">
+      <c r="D31" s="49"/>
+      <c r="E31" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="28" t="s">
+      <c r="G31" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="H31" s="29"/>
-      <c r="I31" s="26" t="s">
+      <c r="H31" s="49"/>
+      <c r="I31" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="K31" s="26" t="s">
+      <c r="K31" s="41" t="s">
         <v>50</v>
       </c>
       <c r="L31" s="2"/>
@@ -1942,25 +1942,25 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" spans="1:23" s="1" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="17" t="s">
         <v>49</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="17" t="s">
         <v>48</v>
       </c>
       <c r="H32" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -2000,19 +2000,19 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2027,19 +2027,19 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="38"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2054,19 +2054,19 @@
       <c r="W35" s="2"/>
     </row>
     <row r="36" spans="1:23" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -2081,19 +2081,19 @@
       <c r="W36" s="2"/>
     </row>
     <row r="37" spans="1:23" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2129,11 +2129,11 @@
     <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="32"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="18"/>
       <c r="H39" s="16" t="s">
         <v>36</v>
@@ -2157,11 +2157,11 @@
     <row r="40" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="36"/>
-      <c r="F40" s="32"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
       <c r="G40" s="18"/>
       <c r="H40" s="16" t="s">
         <v>36</v>
@@ -2185,11 +2185,11 @@
     <row r="41" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="32"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
       <c r="G41" s="18"/>
       <c r="H41" s="16" t="s">
         <v>36</v>
@@ -2214,11 +2214,11 @@
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="41"/>
-      <c r="F42" s="42"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="39"/>
       <c r="G42" s="18"/>
       <c r="H42" s="16" t="s">
         <v>53</v>
@@ -3054,27 +3054,49 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A26:D26"/>
     <mergeCell ref="D42:F42"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:B8"/>
@@ -3091,49 +3113,27 @@
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>